<commit_message>
Corregido capítulo 6 de Juan
</commit_message>
<xml_diff>
--- a/ontology.xlsx
+++ b/ontology.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="579">
   <si>
     <t>id</t>
   </si>
@@ -718,6 +718,9 @@
     <t>per105</t>
   </si>
   <si>
+    <t>padre de Judas Iscariota</t>
+  </si>
+  <si>
     <t>per106</t>
   </si>
   <si>
@@ -1379,6 +1382,9 @@
   </si>
   <si>
     <t>pla55</t>
+  </si>
+  <si>
+    <t>Tiberias</t>
   </si>
   <si>
     <t>pla56</t>
@@ -1876,8 +1882,8 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D106" activeCellId="0" sqref="D106"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B107" activeCellId="0" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2854,505 +2860,511 @@
       <c r="A106" s="0" t="s">
         <v>231</v>
       </c>
+      <c r="B106" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -3374,9 +3386,9 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
+      <selection pane="bottomLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3402,550 +3414,553 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -3985,311 +4000,311 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -4310,8 +4325,8 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4327,132 +4342,132 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -4490,15 +4505,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -4536,18 +4551,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregido el capítulo 9
</commit_message>
<xml_diff>
--- a/ontology.xlsx
+++ b/ontology.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="4" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="9" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="581">
   <si>
     <t>id</t>
   </si>
@@ -1388,6 +1388,9 @@
   </si>
   <si>
     <t>pla56</t>
+  </si>
+  <si>
+    <t>Siloé</t>
   </si>
   <si>
     <t>pla57</t>
@@ -3389,9 +3392,9 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3895,75 +3898,78 @@
       <c r="A57" s="0" t="s">
         <v>455</v>
       </c>
+      <c r="B57" s="0" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -3985,7 +3991,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4003,311 +4009,311 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -4345,135 +4351,135 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -4511,15 +4517,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
   </sheetData>
@@ -4557,18 +4563,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corregido capítulo 15, 16 y 17
</commit_message>
<xml_diff>
--- a/ontology.xlsx
+++ b/ontology.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="8" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="8" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="596">
   <si>
     <t>id</t>
   </si>
@@ -745,9 +745,18 @@
     <t>per109</t>
   </si>
   <si>
+    <t>discípulo amado</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>per110</t>
   </si>
   <si>
+    <t>otro discípulo (no Iscariote)</t>
+  </si>
+  <si>
     <t>per111</t>
   </si>
   <si>
@@ -1777,7 +1786,13 @@
     <t>tim13</t>
   </si>
   <si>
+    <t>muerte de Jesús</t>
+  </si>
+  <si>
     <t>tim14</t>
+  </si>
+  <si>
+    <t>antes del principio</t>
   </si>
   <si>
     <t>tim15</t>
@@ -1989,8 +2004,8 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3008,485 +3023,497 @@
       <c r="A110" s="0" t="s">
         <v>240</v>
       </c>
+      <c r="B110" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -3510,7 +3537,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3536,559 +3563,559 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -4109,8 +4136,8 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4128,323 +4155,323 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4468,8 +4495,8 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4485,138 +4512,144 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>584</v>
+        <v>587</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>585</v>
+        <v>589</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>
@@ -4654,15 +4687,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
     </row>
   </sheetData>
@@ -4700,18 +4733,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nueva ontología como csv
</commit_message>
<xml_diff>
--- a/ontology.xlsx
+++ b/ontology.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="8" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="8" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Personas" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="499">
   <si>
     <t>id</t>
   </si>
@@ -760,9 +760,18 @@
     <t>per111</t>
   </si>
   <si>
+    <t>Malco</t>
+  </si>
+  <si>
     <t>per112</t>
   </si>
   <si>
+    <t>Anás</t>
+  </si>
+  <si>
+    <t>Suegro de Caifas</t>
+  </si>
+  <si>
     <t>per113</t>
   </si>
   <si>
@@ -778,270 +787,6 @@
     <t>per117</t>
   </si>
   <si>
-    <t>per118</t>
-  </si>
-  <si>
-    <t>per119</t>
-  </si>
-  <si>
-    <t>per120</t>
-  </si>
-  <si>
-    <t>per121</t>
-  </si>
-  <si>
-    <t>per122</t>
-  </si>
-  <si>
-    <t>per123</t>
-  </si>
-  <si>
-    <t>per124</t>
-  </si>
-  <si>
-    <t>per125</t>
-  </si>
-  <si>
-    <t>per126</t>
-  </si>
-  <si>
-    <t>per127</t>
-  </si>
-  <si>
-    <t>per128</t>
-  </si>
-  <si>
-    <t>per129</t>
-  </si>
-  <si>
-    <t>per130</t>
-  </si>
-  <si>
-    <t>per131</t>
-  </si>
-  <si>
-    <t>per132</t>
-  </si>
-  <si>
-    <t>per133</t>
-  </si>
-  <si>
-    <t>per134</t>
-  </si>
-  <si>
-    <t>per135</t>
-  </si>
-  <si>
-    <t>per136</t>
-  </si>
-  <si>
-    <t>per137</t>
-  </si>
-  <si>
-    <t>per138</t>
-  </si>
-  <si>
-    <t>per139</t>
-  </si>
-  <si>
-    <t>per140</t>
-  </si>
-  <si>
-    <t>per141</t>
-  </si>
-  <si>
-    <t>per142</t>
-  </si>
-  <si>
-    <t>per143</t>
-  </si>
-  <si>
-    <t>per144</t>
-  </si>
-  <si>
-    <t>per145</t>
-  </si>
-  <si>
-    <t>per146</t>
-  </si>
-  <si>
-    <t>per147</t>
-  </si>
-  <si>
-    <t>per148</t>
-  </si>
-  <si>
-    <t>per149</t>
-  </si>
-  <si>
-    <t>per150</t>
-  </si>
-  <si>
-    <t>per151</t>
-  </si>
-  <si>
-    <t>per152</t>
-  </si>
-  <si>
-    <t>per153</t>
-  </si>
-  <si>
-    <t>per154</t>
-  </si>
-  <si>
-    <t>per155</t>
-  </si>
-  <si>
-    <t>per156</t>
-  </si>
-  <si>
-    <t>per157</t>
-  </si>
-  <si>
-    <t>per158</t>
-  </si>
-  <si>
-    <t>per159</t>
-  </si>
-  <si>
-    <t>per160</t>
-  </si>
-  <si>
-    <t>per161</t>
-  </si>
-  <si>
-    <t>per162</t>
-  </si>
-  <si>
-    <t>per163</t>
-  </si>
-  <si>
-    <t>per164</t>
-  </si>
-  <si>
-    <t>per165</t>
-  </si>
-  <si>
-    <t>per166</t>
-  </si>
-  <si>
-    <t>per167</t>
-  </si>
-  <si>
-    <t>per168</t>
-  </si>
-  <si>
-    <t>per169</t>
-  </si>
-  <si>
-    <t>per170</t>
-  </si>
-  <si>
-    <t>per171</t>
-  </si>
-  <si>
-    <t>per172</t>
-  </si>
-  <si>
-    <t>per173</t>
-  </si>
-  <si>
-    <t>per174</t>
-  </si>
-  <si>
-    <t>per175</t>
-  </si>
-  <si>
-    <t>per176</t>
-  </si>
-  <si>
-    <t>per177</t>
-  </si>
-  <si>
-    <t>per178</t>
-  </si>
-  <si>
-    <t>per179</t>
-  </si>
-  <si>
-    <t>per180</t>
-  </si>
-  <si>
-    <t>per181</t>
-  </si>
-  <si>
-    <t>per182</t>
-  </si>
-  <si>
-    <t>per183</t>
-  </si>
-  <si>
-    <t>per184</t>
-  </si>
-  <si>
-    <t>per185</t>
-  </si>
-  <si>
-    <t>per186</t>
-  </si>
-  <si>
-    <t>per187</t>
-  </si>
-  <si>
-    <t>per188</t>
-  </si>
-  <si>
-    <t>per189</t>
-  </si>
-  <si>
-    <t>per190</t>
-  </si>
-  <si>
-    <t>per191</t>
-  </si>
-  <si>
-    <t>per192</t>
-  </si>
-  <si>
-    <t>per193</t>
-  </si>
-  <si>
-    <t>per194</t>
-  </si>
-  <si>
-    <t>per195</t>
-  </si>
-  <si>
-    <t>per196</t>
-  </si>
-  <si>
-    <t>per197</t>
-  </si>
-  <si>
-    <t>per198</t>
-  </si>
-  <si>
-    <t>per199</t>
-  </si>
-  <si>
-    <t>per200</t>
-  </si>
-  <si>
-    <t>per201</t>
-  </si>
-  <si>
-    <t>per202</t>
-  </si>
-  <si>
-    <t>per203</t>
-  </si>
-  <si>
-    <t>per204</t>
-  </si>
-  <si>
-    <t>per205</t>
-  </si>
-  <si>
     <t>pla1</t>
   </si>
   <si>
@@ -1423,6 +1168,9 @@
     <t>pla58</t>
   </si>
   <si>
+    <t>Cedrón</t>
+  </si>
+  <si>
     <t>pla59</t>
   </si>
   <si>
@@ -1438,27 +1186,6 @@
     <t>pla63</t>
   </si>
   <si>
-    <t>pla64</t>
-  </si>
-  <si>
-    <t>pla65</t>
-  </si>
-  <si>
-    <t>pla66</t>
-  </si>
-  <si>
-    <t>pla67</t>
-  </si>
-  <si>
-    <t>pla68</t>
-  </si>
-  <si>
-    <t>pla69</t>
-  </si>
-  <si>
-    <t>pla70</t>
-  </si>
-  <si>
     <t>org1</t>
   </si>
   <si>
@@ -1672,25 +1399,115 @@
     <t>org35</t>
   </si>
   <si>
-    <t>org36</t>
-  </si>
-  <si>
-    <t>org37</t>
-  </si>
-  <si>
-    <t>org38</t>
-  </si>
-  <si>
-    <t>org39</t>
-  </si>
-  <si>
-    <t>org40</t>
-  </si>
-  <si>
-    <t>org41</t>
-  </si>
-  <si>
-    <t>org42</t>
+    <t>tim1</t>
+  </si>
+  <si>
+    <t>tercer Día</t>
+  </si>
+  <si>
+    <t>tim2</t>
+  </si>
+  <si>
+    <t>Día del juicio; fin del mundo;</t>
+  </si>
+  <si>
+    <t>Tribulación de aquellos Días; fin</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>tim3</t>
+  </si>
+  <si>
+    <t>principio del mundo</t>
+  </si>
+  <si>
+    <t>tim4</t>
+  </si>
+  <si>
+    <t>Días de Noé</t>
+  </si>
+  <si>
+    <t>tim5</t>
+  </si>
+  <si>
+    <t>Pascua</t>
+  </si>
+  <si>
+    <t>tim6</t>
+  </si>
+  <si>
+    <t>Día de la fiesta de los panes sin levadura</t>
+  </si>
+  <si>
+    <t>tim7</t>
+  </si>
+  <si>
+    <t>toma de Jesús</t>
+  </si>
+  <si>
+    <t>esta noche</t>
+  </si>
+  <si>
+    <t>Mat.26,34</t>
+  </si>
+  <si>
+    <t>tim8</t>
+  </si>
+  <si>
+    <t>días del Rey Herodes</t>
+  </si>
+  <si>
+    <t>tim9</t>
+  </si>
+  <si>
+    <t>sábado</t>
+  </si>
+  <si>
+    <t>tim10</t>
+  </si>
+  <si>
+    <t>bodas de Caná</t>
+  </si>
+  <si>
+    <t>tim11</t>
+  </si>
+  <si>
+    <t>fiesta de los tabernáculos</t>
+  </si>
+  <si>
+    <t>tim12</t>
+  </si>
+  <si>
+    <t>fiesta de la Dedicación</t>
+  </si>
+  <si>
+    <t>tim13</t>
+  </si>
+  <si>
+    <t>muerte de Jesús</t>
+  </si>
+  <si>
+    <t>tim14</t>
+  </si>
+  <si>
+    <t>antes del principio</t>
+  </si>
+  <si>
+    <t>tim15</t>
+  </si>
+  <si>
+    <t>tim16</t>
+  </si>
+  <si>
+    <t>wor1</t>
+  </si>
+  <si>
+    <t>antiguo testamtento</t>
+  </si>
+  <si>
+    <t>wor2</t>
   </si>
   <si>
     <t>variantes</t>
@@ -1699,115 +1516,7 @@
     <t>comentarios</t>
   </si>
   <si>
-    <t>tim1</t>
-  </si>
-  <si>
-    <t>tercer Día</t>
-  </si>
-  <si>
-    <t>tim2</t>
-  </si>
-  <si>
-    <t>Día del juicio; fin del mundo;</t>
-  </si>
-  <si>
-    <t>Tribulación de aquellos Días; fin</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>tim3</t>
-  </si>
-  <si>
-    <t>principio del mundo</t>
-  </si>
-  <si>
-    <t>tim4</t>
-  </si>
-  <si>
-    <t>Días de Noé</t>
-  </si>
-  <si>
-    <t>tim5</t>
-  </si>
-  <si>
-    <t>Pascua</t>
-  </si>
-  <si>
-    <t>tim6</t>
-  </si>
-  <si>
-    <t>Día de la fiesta de los panes sin levadura</t>
-  </si>
-  <si>
-    <t>tim7</t>
-  </si>
-  <si>
-    <t>toma de Jesús</t>
-  </si>
-  <si>
-    <t>esta noche</t>
-  </si>
-  <si>
-    <t>Mat.26,34</t>
-  </si>
-  <si>
-    <t>tim8</t>
-  </si>
-  <si>
-    <t>días del Rey Herodes</t>
-  </si>
-  <si>
-    <t>tim9</t>
-  </si>
-  <si>
-    <t>sábado</t>
-  </si>
-  <si>
-    <t>tim10</t>
-  </si>
-  <si>
-    <t>bodas de Caná</t>
-  </si>
-  <si>
-    <t>tim11</t>
-  </si>
-  <si>
-    <t>fiesta de los tabernáculos</t>
-  </si>
-  <si>
-    <t>tim12</t>
-  </si>
-  <si>
-    <t>fiesta de la Dedicación</t>
-  </si>
-  <si>
-    <t>tim13</t>
-  </si>
-  <si>
-    <t>muerte de Jesús</t>
-  </si>
-  <si>
-    <t>tim14</t>
-  </si>
-  <si>
-    <t>antes del principio</t>
-  </si>
-  <si>
-    <t>tim15</t>
-  </si>
-  <si>
-    <t>tim16</t>
-  </si>
-  <si>
     <t>top1</t>
-  </si>
-  <si>
-    <t>wor1</t>
-  </si>
-  <si>
-    <t>antiguo testamtento</t>
   </si>
 </sst>
 </file>
@@ -2002,13 +1711,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D234"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A220" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A233" activeCellId="0" sqref="A233"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.71255060728745"/>
@@ -3045,475 +2754,1002 @@
       <c r="A112" s="0" t="s">
         <v>245</v>
       </c>
+      <c r="B112" s="0" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>254</v>
+        <v>260</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>255</v>
+        <v>263</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>256</v>
+        <v>265</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>257</v>
+        <v>267</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>258</v>
+        <v>269</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>259</v>
+        <v>271</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>260</v>
+        <v>273</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>261</v>
+        <v>275</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>262</v>
+        <v>277</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>263</v>
+        <v>279</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>264</v>
+        <v>281</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>265</v>
+        <v>283</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>266</v>
+        <v>285</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>267</v>
+        <v>288</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>268</v>
+        <v>290</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>269</v>
+        <v>292</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>270</v>
+        <v>295</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>271</v>
+        <v>298</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>272</v>
+        <v>300</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>273</v>
+        <v>302</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>274</v>
+        <v>304</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>275</v>
+        <v>306</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>276</v>
+        <v>308</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>277</v>
+        <v>310</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>278</v>
+        <v>312</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>279</v>
+        <v>314</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>280</v>
+        <v>316</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>281</v>
+        <v>318</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="D148" s="0" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>282</v>
+        <v>321</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>283</v>
+        <v>323</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>284</v>
+        <v>325</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>285</v>
+        <v>327</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>286</v>
+        <v>329</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>287</v>
+        <v>331</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="D154" s="0" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>288</v>
+        <v>334</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>289</v>
+        <v>336</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>290</v>
+        <v>338</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="C157" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="D157" s="0" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>291</v>
+        <v>342</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="D158" s="0" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>292</v>
+        <v>345</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C159" s="0" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>293</v>
+        <v>348</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>294</v>
+        <v>350</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>295</v>
+        <v>352</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>296</v>
+        <v>354</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>297</v>
+        <v>356</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>298</v>
+        <v>358</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>299</v>
+        <v>360</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>300</v>
+        <v>362</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>301</v>
+        <v>364</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>302</v>
+        <v>366</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>303</v>
+        <v>368</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>304</v>
+        <v>370</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="D171" s="0" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>305</v>
+        <v>373</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>306</v>
+        <v>375</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>307</v>
+        <v>377</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>308</v>
+        <v>379</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>309</v>
+        <v>381</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>310</v>
+        <v>383</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>311</v>
+        <v>384</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>312</v>
+        <v>385</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>313</v>
+        <v>386</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>314</v>
+        <v>387</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>315</v>
+        <v>388</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>316</v>
+        <v>390</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>317</v>
+        <v>392</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="D184" s="0" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>318</v>
+        <v>395</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>319</v>
+        <v>397</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>320</v>
+        <v>399</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="C187" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="D187" s="0" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>321</v>
+        <v>403</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>322</v>
+        <v>405</v>
+      </c>
+      <c r="B189" s="0" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>323</v>
+        <v>407</v>
+      </c>
+      <c r="B190" s="0" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>324</v>
+        <v>409</v>
+      </c>
+      <c r="B191" s="0" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>325</v>
+        <v>411</v>
+      </c>
+      <c r="B192" s="0" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>326</v>
+        <v>413</v>
+      </c>
+      <c r="B193" s="0" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>327</v>
+        <v>415</v>
+      </c>
+      <c r="B194" s="0" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>328</v>
+        <v>417</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>329</v>
+        <v>419</v>
+      </c>
+      <c r="B196" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="C196" s="0" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>330</v>
+        <v>422</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>331</v>
+        <v>424</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>332</v>
+        <v>426</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>333</v>
+        <v>428</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>334</v>
+        <v>430</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>335</v>
+        <v>432</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>336</v>
+        <v>434</v>
+      </c>
+      <c r="B203" s="0" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>337</v>
+        <v>436</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>338</v>
+        <v>438</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>339</v>
+        <v>440</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="D206" s="0" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="D208" s="0" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="D210" s="0" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C218" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D218" s="0" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B219" s="0" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="B220" s="0" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="B221" s="0" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="B222" s="0" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="B223" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C223" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D223" s="0" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="B224" s="0" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="B225" s="0" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="B226" s="0" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="B229" s="0" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B233" s="0" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -3532,592 +3768,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.71255060728745"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.5748987854251"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>358</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>370</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>377</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>378</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>380</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>399</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>404</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>408</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>412</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>416</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>421</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>423</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>424</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>425</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>427</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>428</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>430</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>433</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>435</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>437</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>439</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>441</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>443</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>445</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>447</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>449</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>451</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>453</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>455</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>458</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>460</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>464</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>478</v>
-      </c>
-    </row>
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4134,349 +3800,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5748987854251"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>479</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>486</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>491</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>492</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>496</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>498</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>500</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>502</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>504</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>506</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>508</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>510</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>511</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>513</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>517</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>519</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>521</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>523</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>525</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>527</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>529</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>531</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>532</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>534</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>536</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>538</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4493,10 +3828,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4504,154 +3839,23 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5748987854251"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>559</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>571</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>573</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>574</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>575</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>577</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>579</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>581</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>583</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>585</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>587</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>589</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>592</v>
-      </c>
-    </row>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4687,15 +3891,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>557</v>
+        <v>496</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>558</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>593</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -4714,7 +3918,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -4733,18 +3937,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>557</v>
+        <v>496</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>594</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>595</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>